<commit_message>
Did line 29: CURL
</commit_message>
<xml_diff>
--- a/devasc_studyplan.xlsx
+++ b/devasc_studyplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Python\dev_net cert work\study_for_ccna_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88092AF4-D7B0-41D4-A44E-58F25E438A2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E186A2-E678-458A-AEF1-CE8B263A61A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6588" yWindow="6564" windowWidth="26268" windowHeight="18372" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="294">
   <si>
     <t>Important notes</t>
   </si>
@@ -1641,7 +1641,7 @@
   <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2001,6 +2001,9 @@
       </c>
       <c r="E23" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>